<commit_message>
TODO: Adicionar Legenda nas Imagens e comentar um pouco sobre cada grafico
</commit_message>
<xml_diff>
--- a/Excel Carros Informações Versão Atualizada.xlsx
+++ b/Excel Carros Informações Versão Atualizada.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ipbejapt-my.sharepoint.com/personal/23919_stu_ipbeja_pt/Documents/Relatórios-Trabalhos/3º ano/1º Semestre/SI/TG1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="871" documentId="8_{9518B53B-B95E-491D-8120-49B2E10E8827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0CB5455C-9A29-4ED2-ADC7-8F956729DBA8}"/>
+  <xr:revisionPtr revIDLastSave="926" documentId="8_{9518B53B-B95E-491D-8120-49B2E10E8827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C5BEFBDD-D3B2-467D-B463-85807D9C46C5}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{7BD9BC15-55B9-47D1-AC59-4301D45DE72F}"/>
   </bookViews>
@@ -13345,11 +13345,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Aceleração</a:t>
+                  <a:t>Aceleração de 0-60</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> (Segundos)</a:t>
+                  <a:t> milhas por hora  (Segundos)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -16998,7 +16998,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>510540</xdr:colOff>
+      <xdr:colOff>510541</xdr:colOff>
       <xdr:row>41</xdr:row>
       <xdr:rowOff>173935</xdr:rowOff>
     </xdr:to>
@@ -17076,7 +17076,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>512669</xdr:colOff>
+      <xdr:colOff>512670</xdr:colOff>
       <xdr:row>48</xdr:row>
       <xdr:rowOff>83821</xdr:rowOff>
     </xdr:to>
@@ -17277,8 +17277,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Ano do Modelo">
@@ -17301,7 +17301,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -17355,8 +17355,8 @@
       <xdr:row>64</xdr:row>
       <xdr:rowOff>89807</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Marca">
@@ -17379,7 +17379,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -17433,8 +17433,8 @@
       <xdr:row>69</xdr:row>
       <xdr:rowOff>21770</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="6" name="País de Origem">
@@ -17457,7 +17457,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -17552,8 +17552,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>188819</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="3" name="Ano do Modelo 1">
@@ -17576,7 +17576,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -17630,8 +17630,8 @@
       <xdr:row>55</xdr:row>
       <xdr:rowOff>179294</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="4" name="Marca 1">
@@ -17654,7 +17654,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -17708,8 +17708,8 @@
       <xdr:row>62</xdr:row>
       <xdr:rowOff>179291</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="País de Origem 1">
@@ -17732,7 +17732,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -18049,6 +18049,10 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -24729,7 +24733,7 @@
         <item t="default"/>
       </items>
     </pivotField>
-    <pivotField axis="axisPage" showAll="0">
+    <pivotField axis="axisPage" multipleItemSelectionAllowed="1" showAll="0">
       <items count="31">
         <item x="3"/>
         <item x="11"/>
@@ -30656,7 +30660,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC9012A2-EF33-4757-9748-3DA9B16A8308}">
   <dimension ref="A1:K393"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
@@ -44443,14 +44447,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692FC03A-49D7-4E77-88FF-CBC235FE6192}">
   <dimension ref="B2:C18"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView topLeftCell="A22" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="P34" sqref="P34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
@@ -44986,7 +44990,7 @@
       <c r="B5" s="2">
         <v>70</v>
       </c>
-      <c r="C5" s="3">
+      <c r="C5">
         <v>147.82758620689654</v>
       </c>
     </row>
@@ -44994,7 +44998,7 @@
       <c r="B6" s="2">
         <v>71</v>
       </c>
-      <c r="C6" s="3">
+      <c r="C6">
         <v>107.03703703703704</v>
       </c>
     </row>
@@ -45002,7 +45006,7 @@
       <c r="B7" s="2">
         <v>72</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7">
         <v>120.17857142857143</v>
       </c>
     </row>
@@ -45010,7 +45014,7 @@
       <c r="B8" s="2">
         <v>73</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8">
         <v>130.47499999999999</v>
       </c>
     </row>
@@ -45018,7 +45022,7 @@
       <c r="B9" s="2">
         <v>74</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9">
         <v>94.230769230769226</v>
       </c>
     </row>
@@ -45026,7 +45030,7 @@
       <c r="B10" s="2">
         <v>75</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10">
         <v>101.06666666666666</v>
       </c>
     </row>
@@ -45034,7 +45038,7 @@
       <c r="B11" s="2">
         <v>76</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11">
         <v>101.11764705882354</v>
       </c>
     </row>
@@ -45042,7 +45046,7 @@
       <c r="B12" s="2">
         <v>77</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12">
         <v>105.07142857142857</v>
       </c>
     </row>
@@ -45050,7 +45054,7 @@
       <c r="B13" s="2">
         <v>78</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13">
         <v>99.694444444444443</v>
       </c>
     </row>
@@ -45058,7 +45062,7 @@
       <c r="B14" s="2">
         <v>79</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14">
         <v>101.20689655172414</v>
       </c>
     </row>
@@ -45066,7 +45070,7 @@
       <c r="B15" s="2">
         <v>80</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15">
         <v>77.481481481481481</v>
       </c>
     </row>
@@ -45074,7 +45078,7 @@
       <c r="B16" s="2">
         <v>81</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16">
         <v>81.035714285714292</v>
       </c>
     </row>
@@ -45082,7 +45086,7 @@
       <c r="B17" s="2">
         <v>82</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17">
         <v>81.466666666666669</v>
       </c>
     </row>
@@ -45090,7 +45094,7 @@
       <c r="B18" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18">
         <v>104.46938775510205</v>
       </c>
     </row>
@@ -45112,7 +45116,7 @@
   <dimension ref="C2:D18"/>
   <sheetViews>
     <sheetView topLeftCell="A35" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="T39" sqref="T39"/>
+      <selection activeCell="F66" sqref="F66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45176,7 +45180,7 @@
       <c r="C5" s="2">
         <v>70</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5">
         <v>12.948275862068966</v>
       </c>
     </row>
@@ -45184,7 +45188,7 @@
       <c r="C6" s="2">
         <v>71</v>
       </c>
-      <c r="D6" s="3">
+      <c r="D6">
         <v>15</v>
       </c>
     </row>
@@ -45192,7 +45196,7 @@
       <c r="C7" s="2">
         <v>72</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7">
         <v>15.125</v>
       </c>
     </row>
@@ -45200,7 +45204,7 @@
       <c r="C8" s="2">
         <v>73</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8">
         <v>14.3125</v>
       </c>
     </row>
@@ -45208,7 +45212,7 @@
       <c r="C9" s="2">
         <v>74</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9">
         <v>16.173076923076923</v>
       </c>
     </row>
@@ -45216,7 +45220,7 @@
       <c r="C10" s="2">
         <v>75</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10">
         <v>16.05</v>
       </c>
     </row>
@@ -45224,7 +45228,7 @@
       <c r="C11" s="2">
         <v>76</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11">
         <v>15.941176470588232</v>
       </c>
     </row>
@@ -45232,7 +45236,7 @@
       <c r="C12" s="2">
         <v>77</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12">
         <v>15.435714285714285</v>
       </c>
     </row>
@@ -45240,7 +45244,7 @@
       <c r="C13" s="2">
         <v>78</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13">
         <v>15.805555555555552</v>
       </c>
     </row>
@@ -45248,7 +45252,7 @@
       <c r="C14" s="2">
         <v>79</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14">
         <v>15.813793103448274</v>
       </c>
     </row>
@@ -45256,7 +45260,7 @@
       <c r="C15" s="2">
         <v>80</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15">
         <v>17.018518518518519</v>
       </c>
     </row>
@@ -45264,7 +45268,7 @@
       <c r="C16" s="2">
         <v>81</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16">
         <v>16.325000000000006</v>
       </c>
     </row>
@@ -45272,7 +45276,7 @@
       <c r="C17" s="2">
         <v>82</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17">
         <v>16.510000000000002</v>
       </c>
     </row>
@@ -45280,7 +45284,7 @@
       <c r="C18" s="2" t="s">
         <v>300</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18">
         <v>15.541326530612228</v>
       </c>
     </row>

</xml_diff>